<commit_message>
Organizando e modificando planilhas
</commit_message>
<xml_diff>
--- a/documentacao/Planilhas/productBacklog_requisitos.xlsx
+++ b/documentacao/Planilhas/productBacklog_requisitos.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\totem-monitoring\documentacao\Planilhas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laguinho zl\Documents\BandTec\2º Semestre\Projeto e Inovação\totem-monitoring\documentacao\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3378626-BF4A-4364-8D87-A58EC2B2F258}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Requisitos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -251,8 +253,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,14 +263,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,13 +288,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF36FEC2"/>
+        <fgColor rgb="FF4E4A4A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4E4A4A"/>
+        <fgColor rgb="FF9CFEE0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCAFEEE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,72 +525,125 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,8 +653,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCAFEEE"/>
+      <color rgb="FF9CFEE0"/>
+      <color rgb="FF4E4A4A"/>
       <color rgb="FF36FEC2"/>
-      <color rgb="FF4E4A4A"/>
+      <color rgb="FF01CF8F"/>
+      <color rgb="FF01DD99"/>
     </mruColors>
   </colors>
   <extLst>
@@ -860,518 +934,807 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="89" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="84.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="11"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="8">
+      <c r="B4" s="34">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="5">
+      <c r="B5" s="35">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="5">
+      <c r="B6" s="36">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
+      <c r="B7" s="35">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
+      <c r="B8" s="36">
         <v>5</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
+      <c r="B9" s="35">
         <v>6</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
+      <c r="B10" s="36">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="5">
+      <c r="B11" s="35">
         <v>8</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="5">
+      <c r="B12" s="36">
         <v>9</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="5">
+      <c r="B13" s="35">
         <v>10</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="5"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="5"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" s="5"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" s="5"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="5"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="25"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D45" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D46" s="5"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D47" s="5"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D49" s="5"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D50" s="5"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="3"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="31"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="31"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="31"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="31"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="31"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="31"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="31"/>
+      <c r="N26" s="5"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="31"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="31"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="31"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="31"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="31"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="31"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="31"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="31"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="31"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="31"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="31"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="31"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="31"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="31"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="31"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="28"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="31"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="31"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="31"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="31"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="31"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="31"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="31"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="5"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B42:D42"/>
+  <mergeCells count="1">
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD0CF8C-BE43-4F0A-9C04-8F82B8151329}">
+  <dimension ref="B2:D37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="104.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+    </row>
+    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="36"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="36"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="36"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="35"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="35"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="36"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="35"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="36"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="35"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="36"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="35"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="36"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="36"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="35"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="36"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="15"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="36"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="36"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="35"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="36"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="35"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B29:D29"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>